<commit_message>
Timesheets, questions, and class diagram updates
</commit_message>
<xml_diff>
--- a/TimeSheets.xlsx
+++ b/TimeSheets.xlsx
@@ -13,10 +13,10 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="5" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="project_fynbus_time_tracking" localSheetId="1">Sheet2!$A$1:$G$71</definedName>
+    <definedName name="project_fynbus_time_tracking_1" localSheetId="1">Sheet2!$A$1:$G$78</definedName>
     <definedName name="project_fynbus_time_tracking_3" localSheetId="0">Sheet1!$A$1:$G$45</definedName>
     <definedName name="Week1">Sheet1!$E$2:$E$25</definedName>
     <definedName name="Week2">Sheet1!$E$26:$E$57</definedName>
@@ -33,8 +33,8 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="project_fynbus_time_tracking" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="65001" sourceFile="C:\Users\joaml\Downloads\project_fynbus_time_tracking.csv" comma="1">
+  <connection id="1" name="project_fynbus_time_tracking(1)" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr codePage="65001" sourceFile="C:\Users\joaml\Downloads\project_fynbus_time_tracking(1).csv" comma="1">
       <textFields count="7">
         <textField type="MDY"/>
         <textField/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="797" uniqueCount="58">
   <si>
     <t>Date</t>
   </si>
@@ -228,6 +228,15 @@
   </si>
   <si>
     <t>Week 2 Generic Timer</t>
+  </si>
+  <si>
+    <t>Fulfill Offers Test</t>
+  </si>
+  <si>
+    <t>Update ClassDiagram</t>
+  </si>
+  <si>
+    <t>Test for Routes</t>
   </si>
 </sst>
 </file>
@@ -303,7 +312,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="project_fynbus_time_tracking" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="project_fynbus_time_tracking(1)" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -603,10 +612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T71"/>
+  <dimension ref="A1:T78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="A58" sqref="A58:G78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -912,7 +921,7 @@
       </c>
       <c r="N9" s="2">
         <f>SUM(Week3)</f>
-        <v>20.850799999999996</v>
+        <v>22.390999999999998</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.3">
@@ -950,7 +959,7 @@
       </c>
       <c r="N10" s="2">
         <f>N9-$T$5</f>
-        <v>-14.149200000000004</v>
+        <v>-12.609000000000002</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.3">
@@ -2275,16 +2284,16 @@
         <v>8</v>
       </c>
       <c r="D68" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E68">
-        <v>1.4128000000000001</v>
+        <v>1.4861</v>
       </c>
       <c r="F68" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="G68" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
@@ -2298,10 +2307,10 @@
         <v>8</v>
       </c>
       <c r="D69" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E69">
-        <v>5.3900000000000003E-2</v>
+        <v>1.5261</v>
       </c>
       <c r="F69" t="s">
         <v>18</v>
@@ -2324,13 +2333,13 @@
         <v>53</v>
       </c>
       <c r="E70">
-        <v>1.4228000000000001</v>
+        <v>1.4128000000000001</v>
       </c>
       <c r="F70" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G70" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
@@ -2347,13 +2356,174 @@
         <v>53</v>
       </c>
       <c r="E71">
+        <v>5.3900000000000003E-2</v>
+      </c>
+      <c r="F71" t="s">
+        <v>18</v>
+      </c>
+      <c r="G71" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A72" s="1">
+        <v>42816</v>
+      </c>
+      <c r="B72" t="s">
+        <v>7</v>
+      </c>
+      <c r="C72" t="s">
+        <v>8</v>
+      </c>
+      <c r="D72" t="s">
+        <v>53</v>
+      </c>
+      <c r="E72">
+        <v>1.4228000000000001</v>
+      </c>
+      <c r="F72" t="s">
+        <v>12</v>
+      </c>
+      <c r="G72" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A73" s="1">
+        <v>42816</v>
+      </c>
+      <c r="B73" t="s">
+        <v>7</v>
+      </c>
+      <c r="C73" t="s">
+        <v>8</v>
+      </c>
+      <c r="D73" t="s">
+        <v>53</v>
+      </c>
+      <c r="E73">
         <v>4.9200000000000001E-2</v>
       </c>
-      <c r="F71" t="s">
+      <c r="F73" t="s">
         <v>15</v>
       </c>
-      <c r="G71" t="s">
+      <c r="G73" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A74" s="1">
+        <v>42817</v>
+      </c>
+      <c r="B74" t="s">
+        <v>7</v>
+      </c>
+      <c r="C74" t="s">
+        <v>8</v>
+      </c>
+      <c r="D74" t="s">
+        <v>55</v>
+      </c>
+      <c r="E74">
+        <v>0.31669999999999998</v>
+      </c>
+      <c r="F74" t="s">
+        <v>15</v>
+      </c>
+      <c r="G74" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A75" s="1">
+        <v>42817</v>
+      </c>
+      <c r="B75" t="s">
+        <v>7</v>
+      </c>
+      <c r="C75" t="s">
+        <v>8</v>
+      </c>
+      <c r="D75" t="s">
+        <v>56</v>
+      </c>
+      <c r="E75">
+        <v>5.1700000000000003E-2</v>
+      </c>
+      <c r="F75" t="s">
+        <v>9</v>
+      </c>
+      <c r="G75" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A76" s="1">
+        <v>42817</v>
+      </c>
+      <c r="B76" t="s">
+        <v>7</v>
+      </c>
+      <c r="C76" t="s">
+        <v>8</v>
+      </c>
+      <c r="D76" t="s">
+        <v>57</v>
+      </c>
+      <c r="E76">
+        <v>0.37609999999999999</v>
+      </c>
+      <c r="F76" t="s">
+        <v>9</v>
+      </c>
+      <c r="G76" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A77" s="1">
+        <v>42817</v>
+      </c>
+      <c r="B77" t="s">
+        <v>7</v>
+      </c>
+      <c r="C77" t="s">
+        <v>8</v>
+      </c>
+      <c r="D77" t="s">
+        <v>53</v>
+      </c>
+      <c r="E77">
+        <v>0.40670000000000001</v>
+      </c>
+      <c r="F77" t="s">
+        <v>12</v>
+      </c>
+      <c r="G77" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A78" s="1">
+        <v>42817</v>
+      </c>
+      <c r="B78" t="s">
+        <v>7</v>
+      </c>
+      <c r="C78" t="s">
+        <v>8</v>
+      </c>
+      <c r="D78" t="s">
+        <v>53</v>
+      </c>
+      <c r="E78">
+        <v>0.40360000000000001</v>
+      </c>
+      <c r="F78" t="s">
+        <v>9</v>
+      </c>
+      <c r="G78" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -2369,10 +2539,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G71"/>
+  <dimension ref="A1:G78"/>
   <sheetViews>
-    <sheetView topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38:G71"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="A58" sqref="A58:G78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3938,16 +4108,16 @@
         <v>8</v>
       </c>
       <c r="D68" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E68">
-        <v>1.4128000000000001</v>
+        <v>1.4861</v>
       </c>
       <c r="F68" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="G68" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
@@ -3961,10 +4131,10 @@
         <v>8</v>
       </c>
       <c r="D69" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E69">
-        <v>5.3900000000000003E-2</v>
+        <v>1.5261</v>
       </c>
       <c r="F69" t="s">
         <v>18</v>
@@ -3987,13 +4157,13 @@
         <v>53</v>
       </c>
       <c r="E70">
-        <v>1.4228000000000001</v>
+        <v>1.4128000000000001</v>
       </c>
       <c r="F70" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G70" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
@@ -4010,17 +4180,178 @@
         <v>53</v>
       </c>
       <c r="E71">
+        <v>5.3900000000000003E-2</v>
+      </c>
+      <c r="F71" t="s">
+        <v>18</v>
+      </c>
+      <c r="G71" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A72" s="1">
+        <v>42816</v>
+      </c>
+      <c r="B72" t="s">
+        <v>7</v>
+      </c>
+      <c r="C72" t="s">
+        <v>8</v>
+      </c>
+      <c r="D72" t="s">
+        <v>53</v>
+      </c>
+      <c r="E72">
+        <v>1.4228000000000001</v>
+      </c>
+      <c r="F72" t="s">
+        <v>12</v>
+      </c>
+      <c r="G72" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A73" s="1">
+        <v>42816</v>
+      </c>
+      <c r="B73" t="s">
+        <v>7</v>
+      </c>
+      <c r="C73" t="s">
+        <v>8</v>
+      </c>
+      <c r="D73" t="s">
+        <v>53</v>
+      </c>
+      <c r="E73">
         <v>4.9200000000000001E-2</v>
       </c>
-      <c r="F71" t="s">
+      <c r="F73" t="s">
         <v>15</v>
       </c>
-      <c r="G71" t="s">
+      <c r="G73" t="s">
         <v>16</v>
       </c>
     </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A74" s="1">
+        <v>42817</v>
+      </c>
+      <c r="B74" t="s">
+        <v>7</v>
+      </c>
+      <c r="C74" t="s">
+        <v>8</v>
+      </c>
+      <c r="D74" t="s">
+        <v>55</v>
+      </c>
+      <c r="E74">
+        <v>0.31669999999999998</v>
+      </c>
+      <c r="F74" t="s">
+        <v>15</v>
+      </c>
+      <c r="G74" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A75" s="1">
+        <v>42817</v>
+      </c>
+      <c r="B75" t="s">
+        <v>7</v>
+      </c>
+      <c r="C75" t="s">
+        <v>8</v>
+      </c>
+      <c r="D75" t="s">
+        <v>56</v>
+      </c>
+      <c r="E75">
+        <v>5.1700000000000003E-2</v>
+      </c>
+      <c r="F75" t="s">
+        <v>9</v>
+      </c>
+      <c r="G75" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A76" s="1">
+        <v>42817</v>
+      </c>
+      <c r="B76" t="s">
+        <v>7</v>
+      </c>
+      <c r="C76" t="s">
+        <v>8</v>
+      </c>
+      <c r="D76" t="s">
+        <v>57</v>
+      </c>
+      <c r="E76">
+        <v>0.37609999999999999</v>
+      </c>
+      <c r="F76" t="s">
+        <v>9</v>
+      </c>
+      <c r="G76" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A77" s="1">
+        <v>42817</v>
+      </c>
+      <c r="B77" t="s">
+        <v>7</v>
+      </c>
+      <c r="C77" t="s">
+        <v>8</v>
+      </c>
+      <c r="D77" t="s">
+        <v>53</v>
+      </c>
+      <c r="E77">
+        <v>0.40670000000000001</v>
+      </c>
+      <c r="F77" t="s">
+        <v>12</v>
+      </c>
+      <c r="G77" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A78" s="1">
+        <v>42817</v>
+      </c>
+      <c r="B78" t="s">
+        <v>7</v>
+      </c>
+      <c r="C78" t="s">
+        <v>8</v>
+      </c>
+      <c r="D78" t="s">
+        <v>53</v>
+      </c>
+      <c r="E78">
+        <v>0.40360000000000001</v>
+      </c>
+      <c r="F78" t="s">
+        <v>9</v>
+      </c>
+      <c r="G78" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A2:G71">
+  <sortState ref="A2:G78">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added group pictues, and started presentation
</commit_message>
<xml_diff>
--- a/TimeSheets.xlsx
+++ b/TimeSheets.xlsx
@@ -13,14 +13,15 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="5" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="6" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="project_fynbus_time_tracking_1" localSheetId="1">Sheet2!$A$1:$G$78</definedName>
+    <definedName name="project_fynbus_time_tracking_2" localSheetId="1">Sheet2!$A$1:$G$119</definedName>
     <definedName name="project_fynbus_time_tracking_3" localSheetId="0">Sheet1!$A$1:$G$45</definedName>
     <definedName name="Week1">Sheet1!$E$2:$E$25</definedName>
     <definedName name="Week2">Sheet1!$E$26:$E$57</definedName>
-    <definedName name="Week3">Sheet1!$E$58:$E$78</definedName>
+    <definedName name="Week3">Sheet1!$E$58:$E$87</definedName>
+    <definedName name="Week4">Sheet1!$E$88:$E$119</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -33,8 +34,8 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="project_fynbus_time_tracking(1)" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="65001" sourceFile="C:\Users\joaml\Downloads\project_fynbus_time_tracking(1).csv" comma="1">
+  <connection id="1" name="project_fynbus_time_tracking(2)" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr codePage="65001" sourceFile="C:\Users\joaml\Downloads\project_fynbus_time_tracking(2).csv" comma="1">
       <textFields count="7">
         <textField type="MDY"/>
         <textField/>
@@ -63,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="797" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1207" uniqueCount="66">
   <si>
     <t>Date</t>
   </si>
@@ -237,6 +238,30 @@
   </si>
   <si>
     <t>Test for Routes</t>
+  </si>
+  <si>
+    <t>Week 4 Generic Timer</t>
+  </si>
+  <si>
+    <t>Fulfill Integration Tests</t>
+  </si>
+  <si>
+    <t>Fulfill Contractor Tests</t>
+  </si>
+  <si>
+    <t>Fulfill Route Tests</t>
+  </si>
+  <si>
+    <t>Tests for Contractors</t>
+  </si>
+  <si>
+    <t>Integration Tests</t>
+  </si>
+  <si>
+    <t>Week 1/2 Generic Timer</t>
+  </si>
+  <si>
+    <t>SSD</t>
   </si>
 </sst>
 </file>
@@ -312,7 +337,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="project_fynbus_time_tracking(1)" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="project_fynbus_time_tracking(2)" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -612,10 +637,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T78"/>
+  <dimension ref="A1:T119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J67" sqref="J67"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -885,6 +910,9 @@
       <c r="N8">
         <v>3</v>
       </c>
+      <c r="O8">
+        <v>4</v>
+      </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
@@ -921,7 +949,11 @@
       </c>
       <c r="N9" s="2">
         <f>SUM(Week3)</f>
-        <v>25.4178</v>
+        <v>34.927100000000003</v>
+      </c>
+      <c r="O9" s="2">
+        <f>SUM(Week4)</f>
+        <v>35.5518</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.3">
@@ -959,7 +991,11 @@
       </c>
       <c r="N10" s="2">
         <f>N9-$T$5</f>
-        <v>-9.5822000000000003</v>
+        <v>-7.2899999999997078E-2</v>
+      </c>
+      <c r="O10" s="2">
+        <f>O9-$T$5</f>
+        <v>0.55180000000000007</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.3">
@@ -2425,13 +2461,13 @@
         <v>55</v>
       </c>
       <c r="E74">
-        <v>0.31669999999999998</v>
+        <v>2.0491999999999999</v>
       </c>
       <c r="F74" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="G74" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.3">
@@ -2445,16 +2481,16 @@
         <v>8</v>
       </c>
       <c r="D75" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E75">
-        <v>5.1700000000000003E-2</v>
+        <v>2.1036000000000001</v>
       </c>
       <c r="F75" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="G75" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.3">
@@ -2468,10 +2504,10 @@
         <v>8</v>
       </c>
       <c r="D76" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E76">
-        <v>0.37609999999999999</v>
+        <v>0.2586</v>
       </c>
       <c r="F76" t="s">
         <v>9</v>
@@ -2491,16 +2527,16 @@
         <v>8</v>
       </c>
       <c r="D77" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="E77">
-        <v>0.40670000000000001</v>
+        <v>0.1983</v>
       </c>
       <c r="F77" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="G77" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.3">
@@ -2514,16 +2550,959 @@
         <v>8</v>
       </c>
       <c r="D78" t="s">
+        <v>60</v>
+      </c>
+      <c r="E78">
+        <v>0.2</v>
+      </c>
+      <c r="F78" t="s">
+        <v>15</v>
+      </c>
+      <c r="G78" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A79" s="1">
+        <v>42817</v>
+      </c>
+      <c r="B79" t="s">
+        <v>7</v>
+      </c>
+      <c r="C79" t="s">
+        <v>8</v>
+      </c>
+      <c r="D79" t="s">
         <v>53</v>
       </c>
-      <c r="E78">
+      <c r="E79">
+        <v>0.40670000000000001</v>
+      </c>
+      <c r="F79" t="s">
+        <v>12</v>
+      </c>
+      <c r="G79" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A80" s="1">
+        <v>42817</v>
+      </c>
+      <c r="B80" t="s">
+        <v>7</v>
+      </c>
+      <c r="C80" t="s">
+        <v>8</v>
+      </c>
+      <c r="D80" t="s">
+        <v>53</v>
+      </c>
+      <c r="E80">
         <v>0.40360000000000001</v>
       </c>
-      <c r="F78" t="s">
-        <v>9</v>
-      </c>
-      <c r="G78" t="s">
-        <v>10</v>
+      <c r="F80" t="s">
+        <v>9</v>
+      </c>
+      <c r="G80" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A81" s="1">
+        <v>42817</v>
+      </c>
+      <c r="B81" t="s">
+        <v>7</v>
+      </c>
+      <c r="C81" t="s">
+        <v>8</v>
+      </c>
+      <c r="D81" t="s">
+        <v>56</v>
+      </c>
+      <c r="E81">
+        <v>0.86719999999999997</v>
+      </c>
+      <c r="F81" t="s">
+        <v>9</v>
+      </c>
+      <c r="G81" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A82" s="1">
+        <v>42817</v>
+      </c>
+      <c r="B82" t="s">
+        <v>7</v>
+      </c>
+      <c r="C82" t="s">
+        <v>8</v>
+      </c>
+      <c r="D82" t="s">
+        <v>57</v>
+      </c>
+      <c r="E82">
+        <v>0.37609999999999999</v>
+      </c>
+      <c r="F82" t="s">
+        <v>9</v>
+      </c>
+      <c r="G82" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A83" s="1">
+        <v>42817</v>
+      </c>
+      <c r="B83" t="s">
+        <v>7</v>
+      </c>
+      <c r="C83" t="s">
+        <v>8</v>
+      </c>
+      <c r="D83" t="s">
+        <v>57</v>
+      </c>
+      <c r="E83">
+        <v>1.5919000000000001</v>
+      </c>
+      <c r="F83" t="s">
+        <v>12</v>
+      </c>
+      <c r="G83" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A84" s="1">
+        <v>42817</v>
+      </c>
+      <c r="B84" t="s">
+        <v>7</v>
+      </c>
+      <c r="C84" t="s">
+        <v>8</v>
+      </c>
+      <c r="D84" t="s">
+        <v>61</v>
+      </c>
+      <c r="E84">
+        <v>0.61860000000000004</v>
+      </c>
+      <c r="F84" t="s">
+        <v>18</v>
+      </c>
+      <c r="G84" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A85" s="1">
+        <v>42817</v>
+      </c>
+      <c r="B85" t="s">
+        <v>7</v>
+      </c>
+      <c r="C85" t="s">
+        <v>8</v>
+      </c>
+      <c r="D85" t="s">
+        <v>61</v>
+      </c>
+      <c r="E85">
+        <v>0.61670000000000003</v>
+      </c>
+      <c r="F85" t="s">
+        <v>15</v>
+      </c>
+      <c r="G85" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A86" s="1">
+        <v>42817</v>
+      </c>
+      <c r="B86" t="s">
+        <v>7</v>
+      </c>
+      <c r="C86" t="s">
+        <v>8</v>
+      </c>
+      <c r="D86" t="s">
+        <v>62</v>
+      </c>
+      <c r="E86">
+        <v>0.8367</v>
+      </c>
+      <c r="F86" t="s">
+        <v>12</v>
+      </c>
+      <c r="G86" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A87" s="1">
+        <v>42817</v>
+      </c>
+      <c r="B87" t="s">
+        <v>7</v>
+      </c>
+      <c r="C87" t="s">
+        <v>8</v>
+      </c>
+      <c r="D87" t="s">
+        <v>50</v>
+      </c>
+      <c r="E87">
+        <v>0.53690000000000004</v>
+      </c>
+      <c r="F87" t="s">
+        <v>9</v>
+      </c>
+      <c r="G87" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A88" s="1">
+        <v>42821</v>
+      </c>
+      <c r="B88" t="s">
+        <v>7</v>
+      </c>
+      <c r="C88" t="s">
+        <v>8</v>
+      </c>
+      <c r="D88" t="s">
+        <v>58</v>
+      </c>
+      <c r="E88">
+        <v>9.4399999999999998E-2</v>
+      </c>
+      <c r="F88" t="s">
+        <v>9</v>
+      </c>
+      <c r="G88" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A89" s="1">
+        <v>42821</v>
+      </c>
+      <c r="B89" t="s">
+        <v>7</v>
+      </c>
+      <c r="C89" t="s">
+        <v>8</v>
+      </c>
+      <c r="D89" t="s">
+        <v>58</v>
+      </c>
+      <c r="E89">
+        <v>22.636399999999998</v>
+      </c>
+      <c r="F89" t="s">
+        <v>12</v>
+      </c>
+      <c r="G89" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A90" s="1">
+        <v>42821</v>
+      </c>
+      <c r="B90" t="s">
+        <v>7</v>
+      </c>
+      <c r="C90" t="s">
+        <v>8</v>
+      </c>
+      <c r="D90" t="s">
+        <v>63</v>
+      </c>
+      <c r="E90">
+        <v>1.4402999999999999</v>
+      </c>
+      <c r="F90" t="s">
+        <v>18</v>
+      </c>
+      <c r="G90" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A91" s="1">
+        <v>42821</v>
+      </c>
+      <c r="B91" t="s">
+        <v>7</v>
+      </c>
+      <c r="C91" t="s">
+        <v>8</v>
+      </c>
+      <c r="D91" t="s">
+        <v>63</v>
+      </c>
+      <c r="E91">
+        <v>1.4428000000000001</v>
+      </c>
+      <c r="F91" t="s">
+        <v>15</v>
+      </c>
+      <c r="G91" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A92" s="1">
+        <v>42821</v>
+      </c>
+      <c r="B92" t="s">
+        <v>7</v>
+      </c>
+      <c r="C92" t="s">
+        <v>8</v>
+      </c>
+      <c r="D92" t="s">
+        <v>65</v>
+      </c>
+      <c r="E92">
+        <v>0.94750000000000001</v>
+      </c>
+      <c r="F92" t="s">
+        <v>9</v>
+      </c>
+      <c r="G92" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A93" s="1">
+        <v>42821</v>
+      </c>
+      <c r="B93" t="s">
+        <v>7</v>
+      </c>
+      <c r="C93" t="s">
+        <v>8</v>
+      </c>
+      <c r="D93" t="s">
+        <v>65</v>
+      </c>
+      <c r="E93">
+        <v>0.30530000000000002</v>
+      </c>
+      <c r="F93" t="s">
+        <v>12</v>
+      </c>
+      <c r="G93" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A94" s="1">
+        <v>42822</v>
+      </c>
+      <c r="B94" t="s">
+        <v>7</v>
+      </c>
+      <c r="C94" t="s">
+        <v>8</v>
+      </c>
+      <c r="D94" t="s">
+        <v>51</v>
+      </c>
+      <c r="E94">
+        <v>0.43719999999999998</v>
+      </c>
+      <c r="F94" t="s">
+        <v>9</v>
+      </c>
+      <c r="G94" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A95" s="1">
+        <v>42822</v>
+      </c>
+      <c r="B95" t="s">
+        <v>7</v>
+      </c>
+      <c r="C95" t="s">
+        <v>8</v>
+      </c>
+      <c r="D95" t="s">
+        <v>52</v>
+      </c>
+      <c r="E95">
+        <v>0.12859999999999999</v>
+      </c>
+      <c r="F95" t="s">
+        <v>9</v>
+      </c>
+      <c r="G95" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A96" s="1">
+        <v>42822</v>
+      </c>
+      <c r="B96" t="s">
+        <v>7</v>
+      </c>
+      <c r="C96" t="s">
+        <v>8</v>
+      </c>
+      <c r="D96" t="s">
+        <v>61</v>
+      </c>
+      <c r="E96">
+        <v>1.67E-2</v>
+      </c>
+      <c r="F96" t="s">
+        <v>9</v>
+      </c>
+      <c r="G96" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A97" s="1">
+        <v>42822</v>
+      </c>
+      <c r="B97" t="s">
+        <v>7</v>
+      </c>
+      <c r="C97" t="s">
+        <v>8</v>
+      </c>
+      <c r="D97" t="s">
+        <v>62</v>
+      </c>
+      <c r="E97">
+        <v>0.32719999999999999</v>
+      </c>
+      <c r="F97" t="s">
+        <v>12</v>
+      </c>
+      <c r="G97" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A98" s="1">
+        <v>42822</v>
+      </c>
+      <c r="B98" t="s">
+        <v>7</v>
+      </c>
+      <c r="C98" t="s">
+        <v>8</v>
+      </c>
+      <c r="D98" t="s">
+        <v>63</v>
+      </c>
+      <c r="E98">
+        <v>0.28220000000000001</v>
+      </c>
+      <c r="F98" t="s">
+        <v>18</v>
+      </c>
+      <c r="G98" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A99" s="1">
+        <v>42822</v>
+      </c>
+      <c r="B99" t="s">
+        <v>7</v>
+      </c>
+      <c r="C99" t="s">
+        <v>8</v>
+      </c>
+      <c r="D99" t="s">
+        <v>63</v>
+      </c>
+      <c r="E99">
+        <v>0.28189999999999998</v>
+      </c>
+      <c r="F99" t="s">
+        <v>15</v>
+      </c>
+      <c r="G99" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A100" s="1">
+        <v>42822</v>
+      </c>
+      <c r="B100" t="s">
+        <v>7</v>
+      </c>
+      <c r="C100" t="s">
+        <v>8</v>
+      </c>
+      <c r="D100" t="s">
+        <v>65</v>
+      </c>
+      <c r="E100">
+        <v>0.13689999999999999</v>
+      </c>
+      <c r="F100" t="s">
+        <v>9</v>
+      </c>
+      <c r="G100" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A101" s="1">
+        <v>42822</v>
+      </c>
+      <c r="B101" t="s">
+        <v>7</v>
+      </c>
+      <c r="C101" t="s">
+        <v>8</v>
+      </c>
+      <c r="D101" t="s">
+        <v>65</v>
+      </c>
+      <c r="E101">
+        <v>0.61970000000000003</v>
+      </c>
+      <c r="F101" t="s">
+        <v>15</v>
+      </c>
+      <c r="G101" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A102" s="1">
+        <v>42822</v>
+      </c>
+      <c r="B102" t="s">
+        <v>7</v>
+      </c>
+      <c r="C102" t="s">
+        <v>8</v>
+      </c>
+      <c r="D102" t="s">
+        <v>65</v>
+      </c>
+      <c r="E102">
+        <v>0.61080000000000001</v>
+      </c>
+      <c r="F102" t="s">
+        <v>18</v>
+      </c>
+      <c r="G102" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A103" s="1">
+        <v>42823</v>
+      </c>
+      <c r="B103" t="s">
+        <v>7</v>
+      </c>
+      <c r="C103" t="s">
+        <v>8</v>
+      </c>
+      <c r="D103" t="s">
+        <v>58</v>
+      </c>
+      <c r="E103">
+        <v>4.7800000000000002E-2</v>
+      </c>
+      <c r="F103" t="s">
+        <v>9</v>
+      </c>
+      <c r="G103" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A104" s="1">
+        <v>42823</v>
+      </c>
+      <c r="B104" t="s">
+        <v>7</v>
+      </c>
+      <c r="C104" t="s">
+        <v>8</v>
+      </c>
+      <c r="D104" t="s">
+        <v>59</v>
+      </c>
+      <c r="E104">
+        <v>1.2143999999999999</v>
+      </c>
+      <c r="F104" t="s">
+        <v>18</v>
+      </c>
+      <c r="G104" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A105" s="1">
+        <v>42823</v>
+      </c>
+      <c r="B105" t="s">
+        <v>7</v>
+      </c>
+      <c r="C105" t="s">
+        <v>8</v>
+      </c>
+      <c r="D105" t="s">
+        <v>59</v>
+      </c>
+      <c r="E105">
+        <v>1.5667</v>
+      </c>
+      <c r="F105" t="s">
+        <v>15</v>
+      </c>
+      <c r="G105" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A106" s="1">
+        <v>42823</v>
+      </c>
+      <c r="B106" t="s">
+        <v>7</v>
+      </c>
+      <c r="C106" t="s">
+        <v>8</v>
+      </c>
+      <c r="D106" t="s">
+        <v>60</v>
+      </c>
+      <c r="E106">
+        <v>0.31609999999999999</v>
+      </c>
+      <c r="F106" t="s">
+        <v>9</v>
+      </c>
+      <c r="G106" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A107" s="1">
+        <v>42823</v>
+      </c>
+      <c r="B107" t="s">
+        <v>7</v>
+      </c>
+      <c r="C107" t="s">
+        <v>8</v>
+      </c>
+      <c r="D107" t="s">
+        <v>51</v>
+      </c>
+      <c r="E107">
+        <v>2.69E-2</v>
+      </c>
+      <c r="F107" t="s">
+        <v>12</v>
+      </c>
+      <c r="G107" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A108" s="1">
+        <v>42823</v>
+      </c>
+      <c r="B108" t="s">
+        <v>7</v>
+      </c>
+      <c r="C108" t="s">
+        <v>8</v>
+      </c>
+      <c r="D108" t="s">
+        <v>52</v>
+      </c>
+      <c r="E108">
+        <v>2.69E-2</v>
+      </c>
+      <c r="F108" t="s">
+        <v>12</v>
+      </c>
+      <c r="G108" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A109" s="1">
+        <v>42823</v>
+      </c>
+      <c r="B109" t="s">
+        <v>7</v>
+      </c>
+      <c r="C109" t="s">
+        <v>8</v>
+      </c>
+      <c r="D109" t="s">
+        <v>53</v>
+      </c>
+      <c r="E109">
+        <v>7.5300000000000006E-2</v>
+      </c>
+      <c r="F109" t="s">
+        <v>12</v>
+      </c>
+      <c r="G109" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A110" s="1">
+        <v>42823</v>
+      </c>
+      <c r="B110" t="s">
+        <v>7</v>
+      </c>
+      <c r="C110" t="s">
+        <v>8</v>
+      </c>
+      <c r="D110" t="s">
+        <v>56</v>
+      </c>
+      <c r="E110">
+        <v>0.45529999999999998</v>
+      </c>
+      <c r="F110" t="s">
+        <v>9</v>
+      </c>
+      <c r="G110" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A111" s="1">
+        <v>42823</v>
+      </c>
+      <c r="B111" t="s">
+        <v>7</v>
+      </c>
+      <c r="C111" t="s">
+        <v>8</v>
+      </c>
+      <c r="D111" t="s">
+        <v>56</v>
+      </c>
+      <c r="E111">
+        <v>1.5153000000000001</v>
+      </c>
+      <c r="F111" t="s">
+        <v>12</v>
+      </c>
+      <c r="G111" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A112" s="1">
+        <v>42823</v>
+      </c>
+      <c r="B112" t="s">
+        <v>7</v>
+      </c>
+      <c r="C112" t="s">
+        <v>8</v>
+      </c>
+      <c r="D112" t="s">
+        <v>57</v>
+      </c>
+      <c r="E112">
+        <v>3.4200000000000001E-2</v>
+      </c>
+      <c r="F112" t="s">
+        <v>12</v>
+      </c>
+      <c r="G112" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A113" s="1">
+        <v>42824</v>
+      </c>
+      <c r="B113" t="s">
+        <v>7</v>
+      </c>
+      <c r="C113" t="s">
+        <v>8</v>
+      </c>
+      <c r="D113" t="s">
+        <v>58</v>
+      </c>
+      <c r="E113">
+        <v>7.7200000000000005E-2</v>
+      </c>
+      <c r="F113" t="s">
+        <v>9</v>
+      </c>
+      <c r="G113" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A114" s="1">
+        <v>42824</v>
+      </c>
+      <c r="B114" t="s">
+        <v>7</v>
+      </c>
+      <c r="C114" t="s">
+        <v>8</v>
+      </c>
+      <c r="D114" t="s">
+        <v>59</v>
+      </c>
+      <c r="E114">
+        <v>1.67E-2</v>
+      </c>
+      <c r="F114" t="s">
+        <v>18</v>
+      </c>
+      <c r="G114" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A115" s="1">
+        <v>42824</v>
+      </c>
+      <c r="B115" t="s">
+        <v>7</v>
+      </c>
+      <c r="C115" t="s">
+        <v>8</v>
+      </c>
+      <c r="D115" t="s">
+        <v>55</v>
+      </c>
+      <c r="E115">
+        <v>0.28810000000000002</v>
+      </c>
+      <c r="F115" t="s">
+        <v>9</v>
+      </c>
+      <c r="G115" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A116" s="1">
+        <v>42824</v>
+      </c>
+      <c r="B116" t="s">
+        <v>7</v>
+      </c>
+      <c r="C116" t="s">
+        <v>8</v>
+      </c>
+      <c r="D116" t="s">
+        <v>60</v>
+      </c>
+      <c r="E116">
+        <v>4.19E-2</v>
+      </c>
+      <c r="F116" t="s">
+        <v>9</v>
+      </c>
+      <c r="G116" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A117" s="1">
+        <v>42824</v>
+      </c>
+      <c r="B117" t="s">
+        <v>7</v>
+      </c>
+      <c r="C117" t="s">
+        <v>8</v>
+      </c>
+      <c r="D117" t="s">
+        <v>56</v>
+      </c>
+      <c r="E117">
+        <v>0.1</v>
+      </c>
+      <c r="F117" t="s">
+        <v>9</v>
+      </c>
+      <c r="G117" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A118" s="1">
+        <v>42824</v>
+      </c>
+      <c r="B118" t="s">
+        <v>7</v>
+      </c>
+      <c r="C118" t="s">
+        <v>8</v>
+      </c>
+      <c r="D118" t="s">
+        <v>56</v>
+      </c>
+      <c r="E118">
+        <v>1.9400000000000001E-2</v>
+      </c>
+      <c r="F118" t="s">
+        <v>12</v>
+      </c>
+      <c r="G118" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A119" s="1">
+        <v>42824</v>
+      </c>
+      <c r="B119" t="s">
+        <v>7</v>
+      </c>
+      <c r="C119" t="s">
+        <v>8</v>
+      </c>
+      <c r="D119" t="s">
+        <v>62</v>
+      </c>
+      <c r="E119">
+        <v>2.1700000000000001E-2</v>
+      </c>
+      <c r="F119" t="s">
+        <v>12</v>
+      </c>
+      <c r="G119" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -2539,10 +3518,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G78"/>
+  <dimension ref="A1:G119"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58:G78"/>
+    <sheetView topLeftCell="A92" workbookViewId="0">
+      <selection activeCell="A74" sqref="A74:G119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2551,7 +3530,7 @@
     <col min="2" max="2" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.21875" bestFit="1" customWidth="1"/>
   </cols>
@@ -3763,7 +4742,7 @@
         <v>8</v>
       </c>
       <c r="D53" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="E53">
         <v>1.2153</v>
@@ -3786,7 +4765,7 @@
         <v>8</v>
       </c>
       <c r="D54" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="E54">
         <v>0.73219999999999996</v>
@@ -3809,7 +4788,7 @@
         <v>8</v>
       </c>
       <c r="D55" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="E55">
         <v>0.52190000000000003</v>
@@ -3832,7 +4811,7 @@
         <v>8</v>
       </c>
       <c r="D56" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="E56">
         <v>0.46810000000000002</v>
@@ -3855,7 +4834,7 @@
         <v>8</v>
       </c>
       <c r="D57" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="E57">
         <v>0.48170000000000002</v>
@@ -3878,10 +4857,10 @@
         <v>8</v>
       </c>
       <c r="D58" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E58">
-        <v>0.1386</v>
+        <v>2.2425000000000002</v>
       </c>
       <c r="F58" t="s">
         <v>9</v>
@@ -3901,10 +4880,10 @@
         <v>8</v>
       </c>
       <c r="D59" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E59">
-        <v>2.2425000000000002</v>
+        <v>1.3332999999999999</v>
       </c>
       <c r="F59" t="s">
         <v>9</v>
@@ -3924,10 +4903,10 @@
         <v>8</v>
       </c>
       <c r="D60" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E60">
-        <v>1.3332999999999999</v>
+        <v>0.1386</v>
       </c>
       <c r="F60" t="s">
         <v>9</v>
@@ -4016,16 +4995,16 @@
         <v>8</v>
       </c>
       <c r="D64" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="E64">
-        <v>1.2121999999999999</v>
+        <v>1.4861</v>
       </c>
       <c r="F64" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G64" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
@@ -4039,16 +5018,16 @@
         <v>8</v>
       </c>
       <c r="D65" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="E65">
-        <v>1.3028</v>
+        <v>1.5261</v>
       </c>
       <c r="F65" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="G65" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
@@ -4062,16 +5041,16 @@
         <v>8</v>
       </c>
       <c r="D66" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E66">
-        <v>1.2646999999999999</v>
+        <v>1.4128000000000001</v>
       </c>
       <c r="F66" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="G66" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
@@ -4085,16 +5064,16 @@
         <v>8</v>
       </c>
       <c r="D67" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E67">
-        <v>1.8794</v>
+        <v>5.3900000000000003E-2</v>
       </c>
       <c r="F67" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="G67" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
@@ -4108,16 +5087,16 @@
         <v>8</v>
       </c>
       <c r="D68" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E68">
-        <v>1.4861</v>
+        <v>1.4228000000000001</v>
       </c>
       <c r="F68" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G68" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
@@ -4131,16 +5110,16 @@
         <v>8</v>
       </c>
       <c r="D69" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E69">
-        <v>1.5261</v>
+        <v>4.9200000000000001E-2</v>
       </c>
       <c r="F69" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G69" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
@@ -4154,16 +5133,16 @@
         <v>8</v>
       </c>
       <c r="D70" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E70">
-        <v>1.4128000000000001</v>
+        <v>1.2121999999999999</v>
       </c>
       <c r="F70" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="G70" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
@@ -4177,16 +5156,16 @@
         <v>8</v>
       </c>
       <c r="D71" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E71">
-        <v>5.3900000000000003E-2</v>
+        <v>1.3028</v>
       </c>
       <c r="F71" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="G71" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
@@ -4200,16 +5179,16 @@
         <v>8</v>
       </c>
       <c r="D72" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E72">
-        <v>1.4228000000000001</v>
+        <v>1.2646999999999999</v>
       </c>
       <c r="F72" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G72" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.3">
@@ -4223,16 +5202,16 @@
         <v>8</v>
       </c>
       <c r="D73" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E73">
-        <v>4.9200000000000001E-2</v>
+        <v>1.8794</v>
       </c>
       <c r="F73" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="G73" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.3">
@@ -4249,13 +5228,13 @@
         <v>55</v>
       </c>
       <c r="E74">
-        <v>0.31669999999999998</v>
+        <v>2.0491999999999999</v>
       </c>
       <c r="F74" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="G74" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.3">
@@ -4269,16 +5248,16 @@
         <v>8</v>
       </c>
       <c r="D75" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E75">
-        <v>5.1700000000000003E-2</v>
+        <v>2.1036000000000001</v>
       </c>
       <c r="F75" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="G75" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.3">
@@ -4292,10 +5271,10 @@
         <v>8</v>
       </c>
       <c r="D76" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E76">
-        <v>0.37609999999999999</v>
+        <v>0.2586</v>
       </c>
       <c r="F76" t="s">
         <v>9</v>
@@ -4315,16 +5294,16 @@
         <v>8</v>
       </c>
       <c r="D77" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="E77">
-        <v>0.40670000000000001</v>
+        <v>0.1983</v>
       </c>
       <c r="F77" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="G77" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.3">
@@ -4338,21 +5317,964 @@
         <v>8</v>
       </c>
       <c r="D78" t="s">
+        <v>60</v>
+      </c>
+      <c r="E78">
+        <v>0.2</v>
+      </c>
+      <c r="F78" t="s">
+        <v>15</v>
+      </c>
+      <c r="G78" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A79" s="1">
+        <v>42817</v>
+      </c>
+      <c r="B79" t="s">
+        <v>7</v>
+      </c>
+      <c r="C79" t="s">
+        <v>8</v>
+      </c>
+      <c r="D79" t="s">
         <v>53</v>
       </c>
-      <c r="E78">
+      <c r="E79">
+        <v>0.40670000000000001</v>
+      </c>
+      <c r="F79" t="s">
+        <v>12</v>
+      </c>
+      <c r="G79" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A80" s="1">
+        <v>42817</v>
+      </c>
+      <c r="B80" t="s">
+        <v>7</v>
+      </c>
+      <c r="C80" t="s">
+        <v>8</v>
+      </c>
+      <c r="D80" t="s">
+        <v>53</v>
+      </c>
+      <c r="E80">
         <v>0.40360000000000001</v>
       </c>
-      <c r="F78" t="s">
-        <v>9</v>
-      </c>
-      <c r="G78" t="s">
-        <v>10</v>
+      <c r="F80" t="s">
+        <v>9</v>
+      </c>
+      <c r="G80" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A81" s="1">
+        <v>42817</v>
+      </c>
+      <c r="B81" t="s">
+        <v>7</v>
+      </c>
+      <c r="C81" t="s">
+        <v>8</v>
+      </c>
+      <c r="D81" t="s">
+        <v>56</v>
+      </c>
+      <c r="E81">
+        <v>0.86719999999999997</v>
+      </c>
+      <c r="F81" t="s">
+        <v>9</v>
+      </c>
+      <c r="G81" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A82" s="1">
+        <v>42817</v>
+      </c>
+      <c r="B82" t="s">
+        <v>7</v>
+      </c>
+      <c r="C82" t="s">
+        <v>8</v>
+      </c>
+      <c r="D82" t="s">
+        <v>57</v>
+      </c>
+      <c r="E82">
+        <v>0.37609999999999999</v>
+      </c>
+      <c r="F82" t="s">
+        <v>9</v>
+      </c>
+      <c r="G82" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A83" s="1">
+        <v>42817</v>
+      </c>
+      <c r="B83" t="s">
+        <v>7</v>
+      </c>
+      <c r="C83" t="s">
+        <v>8</v>
+      </c>
+      <c r="D83" t="s">
+        <v>57</v>
+      </c>
+      <c r="E83">
+        <v>1.5919000000000001</v>
+      </c>
+      <c r="F83" t="s">
+        <v>12</v>
+      </c>
+      <c r="G83" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A84" s="1">
+        <v>42817</v>
+      </c>
+      <c r="B84" t="s">
+        <v>7</v>
+      </c>
+      <c r="C84" t="s">
+        <v>8</v>
+      </c>
+      <c r="D84" t="s">
+        <v>61</v>
+      </c>
+      <c r="E84">
+        <v>0.61860000000000004</v>
+      </c>
+      <c r="F84" t="s">
+        <v>18</v>
+      </c>
+      <c r="G84" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A85" s="1">
+        <v>42817</v>
+      </c>
+      <c r="B85" t="s">
+        <v>7</v>
+      </c>
+      <c r="C85" t="s">
+        <v>8</v>
+      </c>
+      <c r="D85" t="s">
+        <v>61</v>
+      </c>
+      <c r="E85">
+        <v>0.61670000000000003</v>
+      </c>
+      <c r="F85" t="s">
+        <v>15</v>
+      </c>
+      <c r="G85" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A86" s="1">
+        <v>42817</v>
+      </c>
+      <c r="B86" t="s">
+        <v>7</v>
+      </c>
+      <c r="C86" t="s">
+        <v>8</v>
+      </c>
+      <c r="D86" t="s">
+        <v>62</v>
+      </c>
+      <c r="E86">
+        <v>0.8367</v>
+      </c>
+      <c r="F86" t="s">
+        <v>12</v>
+      </c>
+      <c r="G86" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A87" s="1">
+        <v>42817</v>
+      </c>
+      <c r="B87" t="s">
+        <v>7</v>
+      </c>
+      <c r="C87" t="s">
+        <v>8</v>
+      </c>
+      <c r="D87" t="s">
+        <v>50</v>
+      </c>
+      <c r="E87">
+        <v>0.53690000000000004</v>
+      </c>
+      <c r="F87" t="s">
+        <v>9</v>
+      </c>
+      <c r="G87" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A88" s="1">
+        <v>42821</v>
+      </c>
+      <c r="B88" t="s">
+        <v>7</v>
+      </c>
+      <c r="C88" t="s">
+        <v>8</v>
+      </c>
+      <c r="D88" t="s">
+        <v>58</v>
+      </c>
+      <c r="E88">
+        <v>9.4399999999999998E-2</v>
+      </c>
+      <c r="F88" t="s">
+        <v>9</v>
+      </c>
+      <c r="G88" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A89" s="1">
+        <v>42821</v>
+      </c>
+      <c r="B89" t="s">
+        <v>7</v>
+      </c>
+      <c r="C89" t="s">
+        <v>8</v>
+      </c>
+      <c r="D89" t="s">
+        <v>58</v>
+      </c>
+      <c r="E89">
+        <v>22.636399999999998</v>
+      </c>
+      <c r="F89" t="s">
+        <v>12</v>
+      </c>
+      <c r="G89" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A90" s="1">
+        <v>42821</v>
+      </c>
+      <c r="B90" t="s">
+        <v>7</v>
+      </c>
+      <c r="C90" t="s">
+        <v>8</v>
+      </c>
+      <c r="D90" t="s">
+        <v>63</v>
+      </c>
+      <c r="E90">
+        <v>1.4402999999999999</v>
+      </c>
+      <c r="F90" t="s">
+        <v>18</v>
+      </c>
+      <c r="G90" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A91" s="1">
+        <v>42821</v>
+      </c>
+      <c r="B91" t="s">
+        <v>7</v>
+      </c>
+      <c r="C91" t="s">
+        <v>8</v>
+      </c>
+      <c r="D91" t="s">
+        <v>63</v>
+      </c>
+      <c r="E91">
+        <v>1.4428000000000001</v>
+      </c>
+      <c r="F91" t="s">
+        <v>15</v>
+      </c>
+      <c r="G91" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A92" s="1">
+        <v>42821</v>
+      </c>
+      <c r="B92" t="s">
+        <v>7</v>
+      </c>
+      <c r="C92" t="s">
+        <v>8</v>
+      </c>
+      <c r="D92" t="s">
+        <v>65</v>
+      </c>
+      <c r="E92">
+        <v>0.94750000000000001</v>
+      </c>
+      <c r="F92" t="s">
+        <v>9</v>
+      </c>
+      <c r="G92" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A93" s="1">
+        <v>42821</v>
+      </c>
+      <c r="B93" t="s">
+        <v>7</v>
+      </c>
+      <c r="C93" t="s">
+        <v>8</v>
+      </c>
+      <c r="D93" t="s">
+        <v>65</v>
+      </c>
+      <c r="E93">
+        <v>0.30530000000000002</v>
+      </c>
+      <c r="F93" t="s">
+        <v>12</v>
+      </c>
+      <c r="G93" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A94" s="1">
+        <v>42822</v>
+      </c>
+      <c r="B94" t="s">
+        <v>7</v>
+      </c>
+      <c r="C94" t="s">
+        <v>8</v>
+      </c>
+      <c r="D94" t="s">
+        <v>51</v>
+      </c>
+      <c r="E94">
+        <v>0.43719999999999998</v>
+      </c>
+      <c r="F94" t="s">
+        <v>9</v>
+      </c>
+      <c r="G94" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A95" s="1">
+        <v>42822</v>
+      </c>
+      <c r="B95" t="s">
+        <v>7</v>
+      </c>
+      <c r="C95" t="s">
+        <v>8</v>
+      </c>
+      <c r="D95" t="s">
+        <v>52</v>
+      </c>
+      <c r="E95">
+        <v>0.12859999999999999</v>
+      </c>
+      <c r="F95" t="s">
+        <v>9</v>
+      </c>
+      <c r="G95" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A96" s="1">
+        <v>42822</v>
+      </c>
+      <c r="B96" t="s">
+        <v>7</v>
+      </c>
+      <c r="C96" t="s">
+        <v>8</v>
+      </c>
+      <c r="D96" t="s">
+        <v>61</v>
+      </c>
+      <c r="E96">
+        <v>1.67E-2</v>
+      </c>
+      <c r="F96" t="s">
+        <v>9</v>
+      </c>
+      <c r="G96" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A97" s="1">
+        <v>42822</v>
+      </c>
+      <c r="B97" t="s">
+        <v>7</v>
+      </c>
+      <c r="C97" t="s">
+        <v>8</v>
+      </c>
+      <c r="D97" t="s">
+        <v>62</v>
+      </c>
+      <c r="E97">
+        <v>0.32719999999999999</v>
+      </c>
+      <c r="F97" t="s">
+        <v>12</v>
+      </c>
+      <c r="G97" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A98" s="1">
+        <v>42822</v>
+      </c>
+      <c r="B98" t="s">
+        <v>7</v>
+      </c>
+      <c r="C98" t="s">
+        <v>8</v>
+      </c>
+      <c r="D98" t="s">
+        <v>63</v>
+      </c>
+      <c r="E98">
+        <v>0.28220000000000001</v>
+      </c>
+      <c r="F98" t="s">
+        <v>18</v>
+      </c>
+      <c r="G98" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A99" s="1">
+        <v>42822</v>
+      </c>
+      <c r="B99" t="s">
+        <v>7</v>
+      </c>
+      <c r="C99" t="s">
+        <v>8</v>
+      </c>
+      <c r="D99" t="s">
+        <v>63</v>
+      </c>
+      <c r="E99">
+        <v>0.28189999999999998</v>
+      </c>
+      <c r="F99" t="s">
+        <v>15</v>
+      </c>
+      <c r="G99" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A100" s="1">
+        <v>42822</v>
+      </c>
+      <c r="B100" t="s">
+        <v>7</v>
+      </c>
+      <c r="C100" t="s">
+        <v>8</v>
+      </c>
+      <c r="D100" t="s">
+        <v>65</v>
+      </c>
+      <c r="E100">
+        <v>0.13689999999999999</v>
+      </c>
+      <c r="F100" t="s">
+        <v>9</v>
+      </c>
+      <c r="G100" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A101" s="1">
+        <v>42822</v>
+      </c>
+      <c r="B101" t="s">
+        <v>7</v>
+      </c>
+      <c r="C101" t="s">
+        <v>8</v>
+      </c>
+      <c r="D101" t="s">
+        <v>65</v>
+      </c>
+      <c r="E101">
+        <v>0.61970000000000003</v>
+      </c>
+      <c r="F101" t="s">
+        <v>15</v>
+      </c>
+      <c r="G101" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A102" s="1">
+        <v>42822</v>
+      </c>
+      <c r="B102" t="s">
+        <v>7</v>
+      </c>
+      <c r="C102" t="s">
+        <v>8</v>
+      </c>
+      <c r="D102" t="s">
+        <v>65</v>
+      </c>
+      <c r="E102">
+        <v>0.61080000000000001</v>
+      </c>
+      <c r="F102" t="s">
+        <v>18</v>
+      </c>
+      <c r="G102" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A103" s="1">
+        <v>42823</v>
+      </c>
+      <c r="B103" t="s">
+        <v>7</v>
+      </c>
+      <c r="C103" t="s">
+        <v>8</v>
+      </c>
+      <c r="D103" t="s">
+        <v>58</v>
+      </c>
+      <c r="E103">
+        <v>4.7800000000000002E-2</v>
+      </c>
+      <c r="F103" t="s">
+        <v>9</v>
+      </c>
+      <c r="G103" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A104" s="1">
+        <v>42823</v>
+      </c>
+      <c r="B104" t="s">
+        <v>7</v>
+      </c>
+      <c r="C104" t="s">
+        <v>8</v>
+      </c>
+      <c r="D104" t="s">
+        <v>59</v>
+      </c>
+      <c r="E104">
+        <v>1.2143999999999999</v>
+      </c>
+      <c r="F104" t="s">
+        <v>18</v>
+      </c>
+      <c r="G104" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A105" s="1">
+        <v>42823</v>
+      </c>
+      <c r="B105" t="s">
+        <v>7</v>
+      </c>
+      <c r="C105" t="s">
+        <v>8</v>
+      </c>
+      <c r="D105" t="s">
+        <v>59</v>
+      </c>
+      <c r="E105">
+        <v>1.5667</v>
+      </c>
+      <c r="F105" t="s">
+        <v>15</v>
+      </c>
+      <c r="G105" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A106" s="1">
+        <v>42823</v>
+      </c>
+      <c r="B106" t="s">
+        <v>7</v>
+      </c>
+      <c r="C106" t="s">
+        <v>8</v>
+      </c>
+      <c r="D106" t="s">
+        <v>60</v>
+      </c>
+      <c r="E106">
+        <v>0.31609999999999999</v>
+      </c>
+      <c r="F106" t="s">
+        <v>9</v>
+      </c>
+      <c r="G106" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A107" s="1">
+        <v>42823</v>
+      </c>
+      <c r="B107" t="s">
+        <v>7</v>
+      </c>
+      <c r="C107" t="s">
+        <v>8</v>
+      </c>
+      <c r="D107" t="s">
+        <v>51</v>
+      </c>
+      <c r="E107">
+        <v>2.69E-2</v>
+      </c>
+      <c r="F107" t="s">
+        <v>12</v>
+      </c>
+      <c r="G107" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A108" s="1">
+        <v>42823</v>
+      </c>
+      <c r="B108" t="s">
+        <v>7</v>
+      </c>
+      <c r="C108" t="s">
+        <v>8</v>
+      </c>
+      <c r="D108" t="s">
+        <v>52</v>
+      </c>
+      <c r="E108">
+        <v>2.69E-2</v>
+      </c>
+      <c r="F108" t="s">
+        <v>12</v>
+      </c>
+      <c r="G108" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A109" s="1">
+        <v>42823</v>
+      </c>
+      <c r="B109" t="s">
+        <v>7</v>
+      </c>
+      <c r="C109" t="s">
+        <v>8</v>
+      </c>
+      <c r="D109" t="s">
+        <v>53</v>
+      </c>
+      <c r="E109">
+        <v>7.5300000000000006E-2</v>
+      </c>
+      <c r="F109" t="s">
+        <v>12</v>
+      </c>
+      <c r="G109" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A110" s="1">
+        <v>42823</v>
+      </c>
+      <c r="B110" t="s">
+        <v>7</v>
+      </c>
+      <c r="C110" t="s">
+        <v>8</v>
+      </c>
+      <c r="D110" t="s">
+        <v>56</v>
+      </c>
+      <c r="E110">
+        <v>0.45529999999999998</v>
+      </c>
+      <c r="F110" t="s">
+        <v>9</v>
+      </c>
+      <c r="G110" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A111" s="1">
+        <v>42823</v>
+      </c>
+      <c r="B111" t="s">
+        <v>7</v>
+      </c>
+      <c r="C111" t="s">
+        <v>8</v>
+      </c>
+      <c r="D111" t="s">
+        <v>56</v>
+      </c>
+      <c r="E111">
+        <v>1.5153000000000001</v>
+      </c>
+      <c r="F111" t="s">
+        <v>12</v>
+      </c>
+      <c r="G111" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A112" s="1">
+        <v>42823</v>
+      </c>
+      <c r="B112" t="s">
+        <v>7</v>
+      </c>
+      <c r="C112" t="s">
+        <v>8</v>
+      </c>
+      <c r="D112" t="s">
+        <v>57</v>
+      </c>
+      <c r="E112">
+        <v>3.4200000000000001E-2</v>
+      </c>
+      <c r="F112" t="s">
+        <v>12</v>
+      </c>
+      <c r="G112" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A113" s="1">
+        <v>42824</v>
+      </c>
+      <c r="B113" t="s">
+        <v>7</v>
+      </c>
+      <c r="C113" t="s">
+        <v>8</v>
+      </c>
+      <c r="D113" t="s">
+        <v>58</v>
+      </c>
+      <c r="E113">
+        <v>7.7200000000000005E-2</v>
+      </c>
+      <c r="F113" t="s">
+        <v>9</v>
+      </c>
+      <c r="G113" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A114" s="1">
+        <v>42824</v>
+      </c>
+      <c r="B114" t="s">
+        <v>7</v>
+      </c>
+      <c r="C114" t="s">
+        <v>8</v>
+      </c>
+      <c r="D114" t="s">
+        <v>59</v>
+      </c>
+      <c r="E114">
+        <v>1.67E-2</v>
+      </c>
+      <c r="F114" t="s">
+        <v>18</v>
+      </c>
+      <c r="G114" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A115" s="1">
+        <v>42824</v>
+      </c>
+      <c r="B115" t="s">
+        <v>7</v>
+      </c>
+      <c r="C115" t="s">
+        <v>8</v>
+      </c>
+      <c r="D115" t="s">
+        <v>55</v>
+      </c>
+      <c r="E115">
+        <v>0.28810000000000002</v>
+      </c>
+      <c r="F115" t="s">
+        <v>9</v>
+      </c>
+      <c r="G115" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A116" s="1">
+        <v>42824</v>
+      </c>
+      <c r="B116" t="s">
+        <v>7</v>
+      </c>
+      <c r="C116" t="s">
+        <v>8</v>
+      </c>
+      <c r="D116" t="s">
+        <v>60</v>
+      </c>
+      <c r="E116">
+        <v>4.19E-2</v>
+      </c>
+      <c r="F116" t="s">
+        <v>9</v>
+      </c>
+      <c r="G116" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A117" s="1">
+        <v>42824</v>
+      </c>
+      <c r="B117" t="s">
+        <v>7</v>
+      </c>
+      <c r="C117" t="s">
+        <v>8</v>
+      </c>
+      <c r="D117" t="s">
+        <v>56</v>
+      </c>
+      <c r="E117">
+        <v>0.1</v>
+      </c>
+      <c r="F117" t="s">
+        <v>9</v>
+      </c>
+      <c r="G117" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A118" s="1">
+        <v>42824</v>
+      </c>
+      <c r="B118" t="s">
+        <v>7</v>
+      </c>
+      <c r="C118" t="s">
+        <v>8</v>
+      </c>
+      <c r="D118" t="s">
+        <v>56</v>
+      </c>
+      <c r="E118">
+        <v>1.9400000000000001E-2</v>
+      </c>
+      <c r="F118" t="s">
+        <v>12</v>
+      </c>
+      <c r="G118" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A119" s="1">
+        <v>42824</v>
+      </c>
+      <c r="B119" t="s">
+        <v>7</v>
+      </c>
+      <c r="C119" t="s">
+        <v>8</v>
+      </c>
+      <c r="D119" t="s">
+        <v>62</v>
+      </c>
+      <c r="E119">
+        <v>2.1700000000000001E-2</v>
+      </c>
+      <c r="F119" t="s">
+        <v>12</v>
+      </c>
+      <c r="G119" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:G78">
-    <sortCondition ref="A1"/>
+  <sortState ref="A2:G119">
+    <sortCondition ref="A2:A119"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>